<commit_message>
Excel files done Commit
</commit_message>
<xml_diff>
--- a/src/main/java/com/denovo/ExcelData/CloudPos.xlsx
+++ b/src/main/java/com/denovo/ExcelData/CloudPos.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IntelljWorkspaces\src\main\java\com\denovo\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C37B5E-8D2C-4EA0-917A-42FE269F0E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAFFE72-F336-408B-A9C0-D7E6BF4A3366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{411B86E3-5BC8-4162-9D5B-60D77C5E31A0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{411B86E3-5BC8-4162-9D5B-60D77C5E31A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Quick Sale" sheetId="1" r:id="rId1"/>
     <sheet name="QuickSaleWithCustomFee" sheetId="4" r:id="rId2"/>
     <sheet name="QuickSaleWithSurchargeFee" sheetId="5" r:id="rId3"/>
     <sheet name="QPayWithSendlinkCustomFee" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">QPayWithSendlinkCustomFee!$A$1:$AF$2</definedName>
@@ -135,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="86">
   <si>
     <t>Payment Type</t>
   </si>
@@ -378,24 +377,6 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Admin12</t>
-  </si>
-  <si>
-    <t>Admin12345</t>
-  </si>
-  <si>
-    <t>12344</t>
-  </si>
-  <si>
-    <t>2344</t>
   </si>
   <si>
     <t>2.00</t>
@@ -1004,9 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F299F462-4417-4814-8397-3224DFC664BA}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1216,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A9B68C-F020-4045-8C71-A67E7D034E9A}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD2"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1388,7 +1367,9 @@
       <c r="T2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="U2" s="9"/>
+      <c r="U2" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="V2" s="3" t="s">
         <v>42</v>
       </c>
@@ -1424,7 +1405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829EA237-5DDE-46DE-8061-AEC244A004A5}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1569,7 +1550,7 @@
         <v>31</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>40</v>
@@ -1611,10 +1592,10 @@
         <v>10</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="U2" s="9" t="s">
         <v>16</v>
@@ -1629,7 +1610,7 @@
         <v>79</v>
       </c>
       <c r="Y2" s="9" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="Z2" s="9" t="s">
         <v>73</v>
@@ -1638,13 +1619,13 @@
         <v>74</v>
       </c>
       <c r="AB2" s="9" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="AE2" s="9" t="s">
         <v>12</v>
@@ -1664,48 +1645,4 @@
   <pageSetup orientation="portrait" r:id="rId5"/>
   <legacyDrawing r:id="rId6"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8E6626-6C69-4039-AA2E-5FEBF414F292}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="30.453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>